<commit_message>
Adding test for Amazon e-commerce app
</commit_message>
<xml_diff>
--- a/MultiAppFramework/src/main/java/com/DataTables/MainTables/RunManager.xlsx
+++ b/MultiAppFramework/src/main/java/com/DataTables/MainTables/RunManager.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Google" sheetId="1" r:id="rId1"/>
-    <sheet name="Salesforce" sheetId="2" r:id="rId2"/>
+    <sheet name="Amazon" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Test Case</t>
   </si>
@@ -62,6 +62,21 @@
   </si>
   <si>
     <t>Search in google</t>
+  </si>
+  <si>
+    <t>TC01_AmazonLogin</t>
+  </si>
+  <si>
+    <t>Login to Amazon</t>
+  </si>
+  <si>
+    <t>Search in Amazon</t>
+  </si>
+  <si>
+    <t>TC03_AmazonSearch</t>
+  </si>
+  <si>
+    <t>TC02_AmazonFilter</t>
   </si>
 </sst>
 </file>
@@ -371,7 +386,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -381,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,15 +467,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -479,6 +494,45 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>